<commit_message>
edit emergency 22/09 e-cert
</commit_message>
<xml_diff>
--- a/src/public/xlsx/VolunteerCert_Exemple.xlsx
+++ b/src/public/xlsx/VolunteerCert_Exemple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="18768" windowHeight="5555"/>
   </bookViews>
   <sheets>
     <sheet name="volunteer" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t xml:space="preserve">fullname </t>
   </si>
@@ -38,7 +38,19 @@
     <t>gender</t>
   </si>
   <si>
-    <t>dob</t>
+    <r>
+      <t>dob</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(dd/mm/yyyy)</t>
+    </r>
   </si>
   <si>
     <t>email</t>
@@ -81,6 +93,21 @@
   </si>
   <si>
     <t>Volunteer</t>
+  </si>
+  <si>
+    <t>Nguyễn Bảo Gia Trung</t>
+  </si>
+  <si>
+    <t>123456789103</t>
+  </si>
+  <si>
+    <t>20/09/2007</t>
+  </si>
+  <si>
+    <t>test@gmail.yahoo</t>
+  </si>
+  <si>
+    <t>Organizer</t>
   </si>
 </sst>
 </file>
@@ -94,7 +121,7 @@
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +285,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -717,17 +751,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -736,11 +773,17 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" quotePrefix="1">
       <alignment vertical="center"/>
@@ -1278,41 +1321,42 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="34.3333333333333" customWidth="1"/>
-    <col min="2" max="2" width="16.8888888888889" customWidth="1"/>
-    <col min="3" max="3" width="12.2222222222222" customWidth="1"/>
-    <col min="4" max="4" width="17.8888888888889" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="21.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="34.3333333333333" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.8888888888889" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.2222222222222" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.1111111111111" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.6666666666667" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.8888888888889" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="21" spans="1:7">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1320,22 +1364,22 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>19001900</v>
       </c>
       <c r="G2" t="s">
@@ -1343,29 +1387,55 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>36443</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>19001988</v>
       </c>
       <c r="G3" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2">
+        <v>19002988</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" display="test@gmail.yahoo"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>